<commit_message>
lancaster avenue traffic info
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27823"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27909"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C981604-0AA0-472F-BCB2-08A8CB2B855E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1CDA8F3-2EF8-42A0-9AA3-C2CE8FACAEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>School</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Lankenau</t>
+  </si>
+  <si>
+    <t>Daily Traffic Volume</t>
+  </si>
+  <si>
+    <t>Lancaster Ave</t>
+  </si>
+  <si>
+    <t>https://gis.penndot.pa.gov/BPR_PDF_FILES/MAPS/Traffic/Traffic_Volume/Statewide/Statewide_2022_tv.pdf</t>
   </si>
 </sst>
 </file>
@@ -470,18 +479,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -613,7 +622,26 @@
         <v>370</v>
       </c>
     </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>15000</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D19" r:id="rId1" xr:uid="{6FA85F9E-175D-4F82-B59E-DA9AACD19D39}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bryn Mawr Ave traffic data
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27909"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1CDA8F3-2EF8-42A0-9AA3-C2CE8FACAEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{315B6787-7A59-473D-BA4D-FEBBBCBA5ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>School</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>https://gis.penndot.pa.gov/BPR_PDF_FILES/MAPS/Traffic/Traffic_Volume/Statewide/Statewide_2022_tv.pdf</t>
+  </si>
+  <si>
+    <t>Bryn Mawr Ave</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -638,6 +641,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>8100</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D19" r:id="rId1" xr:uid="{6FA85F9E-175D-4F82-B59E-DA9AACD19D39}"/>

</xml_diff>

<commit_message>
bus information, lancaster/bryn mawr aves
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27909"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{315B6787-7A59-473D-BA4D-FEBBBCBA5ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2391995E-7005-49C6-B897-5876C5E54D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>School</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Bryn Mawr Ave</t>
+  </si>
+  <si>
+    <t>105, 106 Bus Stop, Lancaster/Bryn Mawr</t>
+  </si>
+  <si>
+    <t>https://public.tableau.com/app/profile/daniel.sandiford4261/viz/Stop_Summary_Report_Public_1/Ridership_Map_Public?publish=yes</t>
   </si>
 </sst>
 </file>
@@ -482,18 +488,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" customWidth="1"/>
+    <col min="4" max="4" width="113.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -649,9 +655,21 @@
         <v>8100</v>
       </c>
     </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>94</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D19" r:id="rId1" xr:uid="{6FA85F9E-175D-4F82-B59E-DA9AACD19D39}"/>
+    <hyperlink ref="D22" r:id="rId2" xr:uid="{60284274-0CC0-4C60-945A-7347CB16110C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
workbook changes to total vs. unique train trips
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27914"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2391995E-7005-49C6-B897-5876C5E54D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD056FD3-D21A-4D4F-A9CF-A15679C0479E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>School</t>
   </si>
@@ -102,10 +102,22 @@
     <t>Bryn Mawr Ave</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
     <t>105, 106 Bus Stop, Lancaster/Bryn Mawr</t>
   </si>
   <si>
     <t>https://public.tableau.com/app/profile/daniel.sandiford4261/viz/Stop_Summary_Report_Public_1/Ridership_Map_Public?publish=yes</t>
+  </si>
+  <si>
+    <t>R5 Paoli-Thorndale PAO</t>
+  </si>
+  <si>
+    <t>100 Norristown Speed Line</t>
   </si>
 </sst>
 </file>
@@ -488,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -655,15 +667,33 @@
         <v>8100</v>
       </c>
     </row>
+    <row r="21" spans="1:4">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>94</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Princeton, NJ hotel info.
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27916"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD056FD3-D21A-4D4F-A9CF-A15679C0479E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AAAF9D7-4980-4304-BEAC-03814DE361D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>School</t>
   </si>
@@ -118,13 +118,52 @@
   </si>
   <si>
     <t>100 Norristown Speed Line</t>
+  </si>
+  <si>
+    <t>Local Hotels</t>
+  </si>
+  <si>
+    <t>Rooms</t>
+  </si>
+  <si>
+    <t>Bryn Mawr Guest Suites</t>
+  </si>
+  <si>
+    <t>Facebook page</t>
+  </si>
+  <si>
+    <t>Wyndham Alumae House</t>
+  </si>
+  <si>
+    <t>brynmawr.edu</t>
+  </si>
+  <si>
+    <t>Case Study:</t>
+  </si>
+  <si>
+    <t>Princeton, NJ</t>
+  </si>
+  <si>
+    <t>Princeton University</t>
+  </si>
+  <si>
+    <t>Peacock Inn</t>
+  </si>
+  <si>
+    <t>https://www.peacockinn.com/</t>
+  </si>
+  <si>
+    <t>Nassau Inn</t>
+  </si>
+  <si>
+    <t>https://nassauinn.com/rooms/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +178,18 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,9 +213,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -500,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -696,10 +749,97 @@
         <v>28</v>
       </c>
     </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="B35" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>8842</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>16</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <f>157+31</f>
+        <v>188</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D19" r:id="rId1" xr:uid="{6FA85F9E-175D-4F82-B59E-DA9AACD19D39}"/>
     <hyperlink ref="D22" r:id="rId2" xr:uid="{60284274-0CC0-4C60-945A-7347CB16110C}"/>
+    <hyperlink ref="D28" r:id="rId3" display="brynmawr.edu)" xr:uid="{EAE9A133-61D3-4CFD-8A4C-BD76D27B87D0}"/>
+    <hyperlink ref="D39" r:id="rId4" xr:uid="{89ED1FFA-2103-4FAD-9BA3-4F6C2F73F18B}"/>
+    <hyperlink ref="D40" r:id="rId5" xr:uid="{B6BCE093-6F10-475C-B4AF-2744B4D27C02}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Princeton Junction Rail Traffic
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27916"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AAAF9D7-4980-4304-BEAC-03814DE361D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C5A2F38-634D-4E5E-939E-86853BD5E6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>School</t>
   </si>
@@ -102,61 +102,70 @@
     <t>Bryn Mawr Ave</t>
   </si>
   <si>
+    <t>Boardings</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>105, 106 Bus Stop, Lancaster/Bryn Mawr</t>
+  </si>
+  <si>
+    <t>https://public.tableau.com/app/profile/daniel.sandiford4261/viz/Stop_Summary_Report_Public_1/Ridership_Map_Public?publish=yes</t>
+  </si>
+  <si>
+    <t>R5 Paoli-Thorndale PAO</t>
+  </si>
+  <si>
+    <t>100 Norristown Speed Line</t>
+  </si>
+  <si>
+    <t>Local Hotels</t>
+  </si>
+  <si>
+    <t>Rooms</t>
+  </si>
+  <si>
+    <t>Bryn Mawr Guest Suites</t>
+  </si>
+  <si>
+    <t>Facebook page</t>
+  </si>
+  <si>
+    <t>Wyndham Alumae House</t>
+  </si>
+  <si>
+    <t>brynmawr.edu</t>
+  </si>
+  <si>
+    <t>Case Study:</t>
+  </si>
+  <si>
+    <t>Princeton, NJ</t>
+  </si>
+  <si>
+    <t>Princeton University</t>
+  </si>
+  <si>
+    <t>Peacock Inn</t>
+  </si>
+  <si>
+    <t>https://www.peacockinn.com/</t>
+  </si>
+  <si>
+    <t>Nassau Inn</t>
+  </si>
+  <si>
+    <t>https://nassauinn.com/rooms/</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Unique</t>
-  </si>
-  <si>
-    <t>105, 106 Bus Stop, Lancaster/Bryn Mawr</t>
-  </si>
-  <si>
-    <t>https://public.tableau.com/app/profile/daniel.sandiford4261/viz/Stop_Summary_Report_Public_1/Ridership_Map_Public?publish=yes</t>
-  </si>
-  <si>
-    <t>R5 Paoli-Thorndale PAO</t>
-  </si>
-  <si>
-    <t>100 Norristown Speed Line</t>
-  </si>
-  <si>
-    <t>Local Hotels</t>
-  </si>
-  <si>
-    <t>Rooms</t>
-  </si>
-  <si>
-    <t>Bryn Mawr Guest Suites</t>
-  </si>
-  <si>
-    <t>Facebook page</t>
-  </si>
-  <si>
-    <t>Wyndham Alumae House</t>
-  </si>
-  <si>
-    <t>brynmawr.edu</t>
-  </si>
-  <si>
-    <t>Case Study:</t>
-  </si>
-  <si>
-    <t>Princeton, NJ</t>
-  </si>
-  <si>
-    <t>Princeton University</t>
-  </si>
-  <si>
-    <t>Peacock Inn</t>
-  </si>
-  <si>
-    <t>https://www.peacockinn.com/</t>
-  </si>
-  <si>
-    <t>Nassau Inn</t>
-  </si>
-  <si>
-    <t>https://nassauinn.com/rooms/</t>
+    <t>Princeton Junction</t>
+  </si>
+  <si>
+    <t>https://patch.com/new-jersey/livingston/here-are-new-jersey-transit-s-most-least-used-train-stations</t>
   </si>
 </sst>
 </file>
@@ -553,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -743,11 +752,17 @@
       <c r="A23" t="s">
         <v>27</v>
       </c>
+      <c r="B23">
+        <v>576</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>28</v>
       </c>
+      <c r="B24">
+        <v>294</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
@@ -831,6 +846,25 @@
       </c>
       <c r="D40" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>6817</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -840,6 +874,7 @@
     <hyperlink ref="D28" r:id="rId3" display="brynmawr.edu)" xr:uid="{EAE9A133-61D3-4CFD-8A4C-BD76D27B87D0}"/>
     <hyperlink ref="D39" r:id="rId4" xr:uid="{89ED1FFA-2103-4FAD-9BA3-4F6C2F73F18B}"/>
     <hyperlink ref="D40" r:id="rId5" xr:uid="{B6BCE093-6F10-475C-B4AF-2744B4D27C02}"/>
+    <hyperlink ref="D42" r:id="rId6" xr:uid="{C033C60C-A9A3-457F-AA6B-7B944177E798}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Palo Alto, CA case study
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27916"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C5A2F38-634D-4E5E-939E-86853BD5E6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{437365F1-7024-4C66-8C25-57651CF4950F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>School</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>https://patch.com/new-jersey/livingston/here-are-new-jersey-transit-s-most-least-used-train-stations</t>
+  </si>
+  <si>
+    <t>Princeton</t>
+  </si>
+  <si>
+    <t>Palo Alto, CA</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -867,6 +873,19 @@
         <v>44</v>
       </c>
     </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D19" r:id="rId1" xr:uid="{6FA85F9E-175D-4F82-B59E-DA9AACD19D39}"/>

</xml_diff>

<commit_message>
Evanston, IL hotel data, Northwestern attendance
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27921"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FF4EDD8-5BA3-413A-A68A-D44A3667A308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{902F8207-F3E5-4327-A9FA-5CFBD1B08445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>School</t>
   </si>
@@ -199,6 +199,39 @@
   </si>
   <si>
     <t>Evanston, IL</t>
+  </si>
+  <si>
+    <t>Northwestern University</t>
+  </si>
+  <si>
+    <t>Hilton Garden Inn Chicago North Shore</t>
+  </si>
+  <si>
+    <t>https://www.choosechicago.com/listing/hilton-garden-inn-chicago-north-shore-evanston/</t>
+  </si>
+  <si>
+    <t>Hilton Orrington Evanston</t>
+  </si>
+  <si>
+    <t>https://www.hilton.com/en/hotels/ordoehf-hilton-orrington-evanston/events/</t>
+  </si>
+  <si>
+    <t>Graduate Evanston</t>
+  </si>
+  <si>
+    <t>https://www.choosechicago.com/listing/graduate-evanston/</t>
+  </si>
+  <si>
+    <t>Hyatt House Chicago Evanston</t>
+  </si>
+  <si>
+    <t>https://www.hotelplanner.com/Hotels/223659/Reservations-Hyatt-House-Chicago-Evanston-Evanston-1515-Chicago-Ave-60201#HotelName</t>
+  </si>
+  <si>
+    <t>GEM Museum Suites</t>
+  </si>
+  <si>
+    <t>https://www.qantas.com/hotels/properties/1126680-the-gem-museum-suites</t>
   </si>
 </sst>
 </file>
@@ -595,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -923,6 +956,11 @@
         <v>18283</v>
       </c>
     </row>
+    <row r="50" spans="1:4">
+      <c r="B50" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>48</v>
@@ -967,6 +1005,78 @@
     <row r="57" spans="1:4">
       <c r="B57" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>23161</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>178</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>269</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>119</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62">
+        <v>114</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63">
+        <v>71</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64">
+        <f>SUM(B59:B63)</f>
+        <v>751</v>
       </c>
     </row>
   </sheetData>
@@ -980,6 +1090,11 @@
     <hyperlink ref="D51" r:id="rId7" xr:uid="{1236F3BA-5B3D-4974-855D-1A4DF8312DCA}"/>
     <hyperlink ref="D53" r:id="rId8" location=":~:text=Welcome%20to%20Dinah's%20Garden%20Hotel&amp;text=With%20129%20rooms%20and%20suites,from%20the%20usual%20corporate%20experience" xr:uid="{F74271AA-0340-489E-962A-69C49AFD1685}"/>
     <hyperlink ref="D54" r:id="rId9" location="HotelName" xr:uid="{CEB1CCC0-4BEF-452E-9636-03DF433CC929}"/>
+    <hyperlink ref="D59" r:id="rId10" xr:uid="{0BED2C90-736B-4058-9B96-54502BEC351B}"/>
+    <hyperlink ref="D60" r:id="rId11" xr:uid="{E3DB51E0-9F70-4064-93B0-B474940D27AE}"/>
+    <hyperlink ref="D61" r:id="rId12" xr:uid="{BA4D35E0-583B-4351-9A80-B9C28AAB1EC0}"/>
+    <hyperlink ref="D62" r:id="rId13" location="HotelName" xr:uid="{B1FD7750-ADC3-4941-B152-DBBE63F65381}"/>
+    <hyperlink ref="D63" r:id="rId14" xr:uid="{07DADCDB-D518-4A08-B17B-F09CFA0DACC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
delete palo alto ca add clarendon va
</commit_message>
<xml_diff>
--- a/analysis/7North.xlsx
+++ b/analysis/7North.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27927"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF64E52C-685C-4C66-B02C-314625009989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84639102-6C19-4B48-B8F1-6E2701B47216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>School</t>
   </si>
@@ -171,12 +171,6 @@
     <t>Princeton</t>
   </si>
   <si>
-    <t>Palo Alto, CA</t>
-  </si>
-  <si>
-    <t>Stanford</t>
-  </si>
-  <si>
     <t>Homewood Suites</t>
   </si>
   <si>
@@ -235,6 +229,18 @@
   </si>
   <si>
     <t xml:space="preserve">Westfield NJ </t>
+  </si>
+  <si>
+    <t>westfield Inn, BW Signature</t>
+  </si>
+  <si>
+    <t>No major college other than Union Co. Community College</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No inpatient hospital </t>
+  </si>
+  <si>
+    <t>Clarendon VA</t>
   </si>
 </sst>
 </file>
@@ -631,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -944,21 +950,6 @@
         <v>814</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="B51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="B53">
-        <v>18283</v>
-      </c>
-    </row>
     <row r="55" spans="1:4">
       <c r="B55" s="3" t="s">
         <v>1</v>
@@ -966,18 +957,18 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B56">
         <v>138</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B57">
         <v>191</v>
@@ -985,34 +976,34 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B58">
         <v>129</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B59">
         <v>156</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="B62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B63">
         <v>23161</v>
@@ -1020,57 +1011,57 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B64">
         <v>178</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B65">
         <v>269</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B66">
         <v>119</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B67">
         <v>114</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B68">
         <v>71</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1084,7 +1075,30 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>